<commit_message>
Yaw Angle Control Just Finished
</commit_message>
<xml_diff>
--- a/Design/Mechanical/Max Torque Calcs.xlsx
+++ b/Design/Mechanical/Max Torque Calcs.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11310"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11310" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -505,8 +506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -699,4 +700,53 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>3.3519999999999999</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>9.81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>A2*A1</f>
+        <v>32.883119999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>25</v>
+      </c>
+      <c r="B5">
+        <f>(A5-A3)/A1</f>
+        <v>-2.3517661097852023</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>50</v>
+      </c>
+      <c r="B6">
+        <f>(A6-A3)/A1</f>
+        <v>5.106467780429595</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>